<commit_message>
Correct error process hyphen in param value
</commit_message>
<xml_diff>
--- a/test/src/ATTD/Kata Args ATDD sheet.xlsx
+++ b/test/src/ATTD/Kata Args ATDD sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tscott\Documents\AL\Kata\Args\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Jendev\ParameterHandling\test\src\ATTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73FC2D8-27BE-4051-8C53-750E96A0FF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF911E1A-9984-4BD0-BD5B-5FD0F0006587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
@@ -525,119 +525,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -699,6 +586,57 @@
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1162,6 +1100,68 @@
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1176,25 +1176,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{349C639E-D4F0-42BE-A366-DDE5E45A8C38}" name="Table3" displayName="Table3" ref="A1:L17" totalsRowShown="0" headerRowDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{349C639E-D4F0-42BE-A366-DDE5E45A8C38}" name="Table3" displayName="Table3" ref="A1:L17" totalsRowShown="0" headerRowDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A1:L17" xr:uid="{349C639E-D4F0-42BE-A366-DDE5E45A8C38}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{60872961-10DF-4005-9BD6-F3431D7EC4D5}" name="Feature" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{087C65D2-1E68-4E79-BC79-4A5C1AD9121D}" name="Sub Feature" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{13391FBE-2D30-4996-B96D-7A3C45D7B1B0}" name="UI" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{4E83241E-A5EB-4264-8924-38ECBD33AB6B}" name="Positive-negative" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{C6AE30F7-AEE5-4C0D-82FC-09AD2A123B5D}" name="Scenario #" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{52A27CB7-AECE-4BD0-A77E-789A2BA6ACAF}" name="Scenario" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{AD2C7CA8-9621-4005-9994-EB4C41B03407}" name="Given-When-Then (Tag)" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{6336EB7F-CCB5-4142-9382-F3FF1DEF5797}" name="Given-When-Then (Description)" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{10BEEDE9-BC82-425B-9D78-DE9A80579A29}" name="Notes" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{C2905CBE-A863-47BA-AF4C-34025581EA72}" name="ATDD Format" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{60872961-10DF-4005-9BD6-F3431D7EC4D5}" name="Feature" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{087C65D2-1E68-4E79-BC79-4A5C1AD9121D}" name="Sub Feature" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{13391FBE-2D30-4996-B96D-7A3C45D7B1B0}" name="UI" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{4E83241E-A5EB-4264-8924-38ECBD33AB6B}" name="Positive-negative" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{C6AE30F7-AEE5-4C0D-82FC-09AD2A123B5D}" name="Scenario #" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{52A27CB7-AECE-4BD0-A77E-789A2BA6ACAF}" name="Scenario" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{AD2C7CA8-9621-4005-9994-EB4C41B03407}" name="Given-When-Then (Tag)" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{6336EB7F-CCB5-4142-9382-F3FF1DEF5797}" name="Given-When-Then (Description)" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{10BEEDE9-BC82-425B-9D78-DE9A80579A29}" name="Notes" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{C2905CBE-A863-47BA-AF4C-34025581EA72}" name="ATDD Format" dataDxfId="23">
       <calculatedColumnFormula>IF('ATDD Scenarios'!$G2="",IF('ATDD Scenarios'!$F2="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT('ATDD Scenarios'!$A2," ",'ATDD Scenarios'!$B2)),_xlfn.CONCAT("[SCENARIO #",TEXT('ATDD Scenarios'!$E2,"0000"),"] ",'ATDD Scenarios'!$F2)),_xlfn.CONCAT("[",UPPER('ATDD Scenarios'!$G2),"] ",'ATDD Scenarios'!$H2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{BB3870CB-8EF3-48C0-8022-0B24013C74FC}" name="Code Format" dataDxfId="30">
+    <tableColumn id="11" xr3:uid="{BB3870CB-8EF3-48C0-8022-0B24013C74FC}" name="Code Format" dataDxfId="22">
       <calculatedColumnFormula>_xlfn.CONCAT("//",'ATDD Scenarios'!$J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{CDC0E25B-784C-47B9-97EB-4043BDECCD97}" name="ATDD.TestScriptor Format" dataDxfId="29">
+    <tableColumn id="12" xr3:uid="{CDC0E25B-784C-47B9-97EB-4043BDECCD97}" name="ATDD.TestScriptor Format" dataDxfId="21">
       <calculatedColumnFormula>IF('ATDD Scenarios'!$G2="",IF('ATDD Scenarios'!$F2="",IF('ATDD Scenarios'!$A2&lt;&gt;"",_xlfn.CONCAT("Feature '",'ATDD Scenarios'!$A2," ",'ATDD Scenarios'!$B2,"' {"),""),_xlfn.CONCAT("Scenario ",TEXT('ATDD Scenarios'!$E2,"0000")," '",'ATDD Scenarios'!$F2,"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT('ATDD Scenarios'!$G2," '",'ATDD Scenarios'!$H2,"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT('ATDD Scenarios'!$G2," '",'ATDD Scenarios'!$H2,"' }"),_xlfn.CONCAT('ATDD Scenarios'!$G2," '",'ATDD Scenarios'!$H2,"' } }"))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1217,27 +1217,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:L17" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EB12FABE-99EE-4C64-9371-664DA2BC018B}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{C4BF811B-A50B-4F15-ABFB-76F5EF61BAEC}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{CC6D9ED1-342A-442A-A781-19E1B48EC192}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="8">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="20">
+    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="6">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C97F81-45CE-49FB-8C99-7D99767A1766}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2110,7 +2110,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C12 C18:C1048576">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2127,29 +2127,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:E12 E3:E17 D18:E1048576">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" stopIfTrue="1" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2260,7 +2260,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2820,7 +2820,7 @@
     <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2837,18 +2837,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>